<commit_message>
Changes brought to implement temperature into the model. The main change is the adding of a code into preprocessing.py, and the rest of the code has been modified in order to enable this modification. Also, some csv files have been modified (heat demand, powerplants)
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigCY.xlsx
+++ b/ConfigFiles/ConfigCY.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="7425" windowHeight="1815"/>
@@ -11,12 +11,12 @@
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="ReserveParticipation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="161">
   <si>
     <t>Default value</t>
   </si>
@@ -471,10 +471,34 @@
     <t>Load Shedding Cost</t>
   </si>
   <si>
-    <t>Database/PowerPlants/##/2015_heatpump.csv</t>
-  </si>
-  <si>
-    <t>Database/Heat_demand/CY/vassilikos_chp_p2h.csv</t>
+    <t>District heating</t>
+  </si>
+  <si>
+    <t>Total Heat demand</t>
+  </si>
+  <si>
+    <t>These inputs are used to quickly modify the district heating configuration</t>
+  </si>
+  <si>
+    <t>Database/PowerPlants/##/2015_heatpump3.csv</t>
+  </si>
+  <si>
+    <t>HeatLoss</t>
+  </si>
+  <si>
+    <t>Part of DH</t>
+  </si>
+  <si>
+    <t>Percentage [0, 1]</t>
+  </si>
+  <si>
+    <t>Temperature Outside</t>
+  </si>
+  <si>
+    <t>Database/OutsideTemperature/##/NL2050.csv</t>
+  </si>
+  <si>
+    <t>Database/Heat_demand/CY/Vassilikos_CCP2.csv</t>
   </si>
 </sst>
 </file>
@@ -671,7 +695,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -958,13 +982,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H165"/>
+  <dimension ref="A1:H176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
@@ -1169,7 +1193,7 @@
         <v>41</v>
       </c>
       <c r="C32" s="21">
-        <v>42012</v>
+        <v>42019</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>79</v>
@@ -1325,7 +1349,7 @@
         <v>39</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>96</v>
@@ -1589,7 +1613,7 @@
         <v>39</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="D79" s="22" t="s">
         <v>96</v>
@@ -1937,7 +1961,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
@@ -1945,110 +1968,32 @@
     <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="10"/>
-      <c r="C128" s="18"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="1:3" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="1:3" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="10"/>
+      <c r="C139" s="18"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B132" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="C132" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B133" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C133" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B134" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C134" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B135" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C135" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="C136" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B137" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C137" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B138" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="C138" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B139" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="C139" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B140" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="C140" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B141" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="C141" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B142" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="C142" s="26" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" s="27" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C143" s="26" t="b">
         <v>1</v>
@@ -2056,22 +2001,166 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C144" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B145" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C145" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B146" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C146" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B147" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C147" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B148" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C148" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B149" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C149" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B150" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C150" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B151" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C151" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B152" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C152" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B153" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C153" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B154" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C154" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B155" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C144" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" s="27" t="s">
+      <c r="C155" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B156" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C145" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F165" s="2"/>
+      <c r="C156" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="10"/>
+      <c r="C158" s="18"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C161" s="5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C162" s="5">
+        <v>1</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C163" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F176" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2093,9 +2182,9 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C68"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F70:F74 F77:F78 F80:F81"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C112"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C113"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C112 C161"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C113 C162"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114 C163"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C115"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F66"/>
@@ -2111,7 +2200,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F88:G102 C88:C102 C132:C145</xm:sqref>
+          <xm:sqref>F88:G102 C88:C102 C143:C156</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write excel files" prompt="If set to true, one excel file per parameter will be written in the simulation environment directory.">
           <x14:formula1>
@@ -2164,7 +2253,7 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
@@ -2239,7 +2328,7 @@
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="20"/>
   </cols>

</xml_diff>

<commit_message>
Get simple example to run
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigCY.xlsx
+++ b/ConfigFiles/ConfigCY.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="7425" windowHeight="1815"/>
@@ -11,7 +11,7 @@
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="ReserveParticipation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -480,8 +480,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -745,7 +745,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -780,7 +779,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -956,15 +954,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
@@ -977,7 +975,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>58</v>
       </c>
@@ -989,7 +987,7 @@
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -999,8 +997,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="3.75" customHeight="1"/>
+    <row r="4" spans="1:8" ht="43.5" customHeight="1">
       <c r="B4" s="31" t="s">
         <v>63</v>
       </c>
@@ -1011,7 +1009,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="9" customFormat="1" ht="10.5" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -1021,7 +1019,7 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
@@ -1035,7 +1033,7 @@
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
     </row>
-    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="8.25" customHeight="1">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -1044,20 +1042,20 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="9" customFormat="1" ht="17.25" customHeight="1">
       <c r="A8" s="8"/>
       <c r="C8" s="17"/>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1"/>
+    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1"/>
+    <row r="11" spans="1:8" hidden="1"/>
+    <row r="12" spans="1:8" hidden="1"/>
+    <row r="13" spans="1:8" hidden="1"/>
+    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1"/>
+    <row r="15" spans="1:8" hidden="1"/>
+    <row r="16" spans="1:8" hidden="1"/>
+    <row r="17" spans="1:8" hidden="1"/>
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1072,7 +1070,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -1086,7 +1084,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1094,13 +1092,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1114,7 +1112,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
         <v>92</v>
       </c>
@@ -1125,7 +1123,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
         <v>148</v>
       </c>
@@ -1137,17 +1135,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="1.5" hidden="1" customHeight="1"/>
+    <row r="25" spans="1:8" hidden="1"/>
+    <row r="26" spans="1:8" hidden="1"/>
+    <row r="27" spans="1:8" hidden="1"/>
+    <row r="28" spans="1:8" ht="1.5" customHeight="1"/>
+    <row r="29" spans="1:8" ht="9.75" customHeight="1"/>
+    <row r="30" spans="1:8" s="9" customFormat="1">
       <c r="A30" s="8"/>
       <c r="C30" s="17"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -1161,7 +1159,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
         <v>43</v>
       </c>
@@ -1175,7 +1173,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
@@ -1189,7 +1187,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
         <v>52</v>
       </c>
@@ -1200,20 +1198,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1"/>
+    <row r="37" spans="1:8" hidden="1"/>
+    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1"/>
+    <row r="39" spans="1:8" hidden="1"/>
+    <row r="40" spans="1:8" hidden="1"/>
+    <row r="41" spans="1:8" hidden="1"/>
+    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1"/>
+    <row r="43" spans="1:8" hidden="1"/>
+    <row r="44" spans="1:8" hidden="1"/>
+    <row r="45" spans="1:8" s="9" customFormat="1" ht="16.5" customHeight="1">
       <c r="A45" s="8"/>
       <c r="C45" s="17"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
         <v>54</v>
       </c>
@@ -1227,7 +1225,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -1242,7 +1240,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>67</v>
       </c>
@@ -1257,7 +1255,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="12.75" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>139</v>
       </c>
@@ -1269,25 +1267,25 @@
       </c>
       <c r="D49" s="14"/>
     </row>
-    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:8" s="11" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1"/>
+    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1"/>
+    <row r="52" spans="1:8" hidden="1"/>
+    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1"/>
+    <row r="54" spans="1:8" hidden="1"/>
+    <row r="55" spans="1:8" hidden="1"/>
+    <row r="56" spans="1:8" hidden="1"/>
+    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1"/>
+    <row r="58" spans="1:8" hidden="1"/>
+    <row r="59" spans="1:8" hidden="1"/>
+    <row r="60" spans="1:8" s="11" customFormat="1" ht="9.75" customHeight="1">
       <c r="A60" s="10"/>
       <c r="C60" s="18"/>
     </row>
-    <row r="61" spans="1:8" s="9" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="9" customFormat="1" ht="9.75" customHeight="1">
       <c r="A61" s="8"/>
       <c r="C61" s="17"/>
     </row>
-    <row r="62" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" s="16" customFormat="1">
       <c r="A62" s="15" t="s">
         <v>2</v>
       </c>
@@ -1302,7 +1300,7 @@
       </c>
       <c r="H62" s="12"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
@@ -1317,7 +1315,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -1334,7 +1332,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="2" t="s">
         <v>40</v>
       </c>
@@ -1348,7 +1346,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="2" t="s">
         <v>44</v>
       </c>
@@ -1369,7 +1367,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="2" t="s">
         <v>53</v>
       </c>
@@ -1386,7 +1384,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="2" t="s">
         <v>100</v>
       </c>
@@ -1403,7 +1401,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="2" t="s">
         <v>143</v>
       </c>
@@ -1418,7 +1416,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="2" t="s">
         <v>135</v>
       </c>
@@ -1434,7 +1432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="2" t="s">
         <v>102</v>
       </c>
@@ -1452,7 +1450,7 @@
         <v>10.62</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="2" t="s">
         <v>68</v>
       </c>
@@ -1473,7 +1471,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
@@ -1493,7 +1491,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="16.5" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>136</v>
       </c>
@@ -1513,7 +1511,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="2" t="s">
         <v>137</v>
       </c>
@@ -1531,7 +1529,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="2" t="s">
         <v>141</v>
       </c>
@@ -1543,7 +1541,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="2" t="s">
         <v>146</v>
       </c>
@@ -1561,7 +1559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="2" t="s">
         <v>147</v>
       </c>
@@ -1581,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="2" t="s">
         <v>145</v>
       </c>
@@ -1595,7 +1593,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="2" t="s">
         <v>149</v>
       </c>
@@ -1613,7 +1611,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
         <v>150</v>
       </c>
@@ -1631,21 +1629,21 @@
         <v>400</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:6" s="11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="9.75" hidden="1" customHeight="1"/>
+    <row r="83" spans="1:6" ht="15.75" hidden="1" customHeight="1"/>
+    <row r="84" spans="1:6" ht="9.75" customHeight="1"/>
+    <row r="85" spans="1:6" s="11" customFormat="1" ht="13.5" customHeight="1">
       <c r="A85" s="10"/>
       <c r="C85" s="18"/>
     </row>
-    <row r="86" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="13.5" customHeight="1"/>
+    <row r="87" spans="1:6" ht="13.5" customHeight="1">
       <c r="A87" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="29" t="s">
         <v>57</v>
       </c>
@@ -1662,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="29"/>
       <c r="B89" s="7" t="s">
         <v>5</v>
@@ -1677,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="29"/>
       <c r="B90" s="7" t="s">
         <v>6</v>
@@ -1692,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="29"/>
       <c r="B91" s="7" t="s">
         <v>33</v>
@@ -1707,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="29"/>
       <c r="B92" s="7" t="s">
         <v>17</v>
@@ -1722,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="29"/>
       <c r="B93" s="7" t="s">
         <v>7</v>
@@ -1737,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="29"/>
       <c r="B94" s="7" t="s">
         <v>9</v>
@@ -1752,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="29"/>
       <c r="B95" s="7" t="s">
         <v>8</v>
@@ -1767,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="29"/>
       <c r="B96" s="7" t="s">
         <v>10</v>
@@ -1782,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="29"/>
       <c r="B97" s="7" t="s">
         <v>12</v>
@@ -1797,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="29"/>
       <c r="B98" s="7" t="s">
         <v>13</v>
@@ -1812,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="29"/>
       <c r="B99" s="7" t="s">
         <v>30</v>
@@ -1827,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="29"/>
       <c r="B100" s="7" t="s">
         <v>14</v>
@@ -1842,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="29"/>
       <c r="B101" s="7" t="s">
         <v>15</v>
@@ -1857,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102" s="29"/>
       <c r="B102" s="7" t="s">
         <v>21</v>
@@ -1872,22 +1870,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:6" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="11.25" customHeight="1"/>
+    <row r="104" spans="1:6" hidden="1"/>
+    <row r="105" spans="1:6" ht="0.75" hidden="1" customHeight="1"/>
+    <row r="106" spans="1:6" hidden="1"/>
+    <row r="107" spans="1:6" hidden="1"/>
+    <row r="108" spans="1:6" ht="10.5" customHeight="1"/>
+    <row r="109" spans="1:6" s="11" customFormat="1">
       <c r="A109" s="10"/>
       <c r="C109" s="18"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6">
       <c r="A111" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6">
       <c r="A112" s="15" t="s">
         <v>2</v>
       </c>
@@ -1898,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8">
       <c r="A113" s="2" t="s">
         <v>81</v>
       </c>
@@ -1912,7 +1910,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8">
       <c r="A114" s="2" t="s">
         <v>82</v>
       </c>
@@ -1926,7 +1924,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8">
       <c r="A115" s="2" t="s">
         <v>84</v>
       </c>
@@ -1937,28 +1935,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="22.5" customHeight="1"/>
+    <row r="117" spans="1:8" hidden="1"/>
+    <row r="118" spans="1:8" hidden="1"/>
+    <row r="119" spans="1:8" hidden="1"/>
+    <row r="120" spans="1:8" hidden="1"/>
+    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1"/>
+    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1"/>
+    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1"/>
+    <row r="124" spans="1:8" ht="1.5" customHeight="1"/>
+    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1"/>
+    <row r="126" spans="1:8" hidden="1"/>
+    <row r="127" spans="1:8" hidden="1"/>
+    <row r="128" spans="1:8" s="11" customFormat="1">
       <c r="A128" s="10"/>
       <c r="C128" s="18"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3">
       <c r="A130" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3">
       <c r="B132" s="27" t="s">
         <v>104</v>
       </c>
@@ -1966,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3">
       <c r="B133" s="27" t="s">
         <v>105</v>
       </c>
@@ -1974,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3">
       <c r="B134" s="27" t="s">
         <v>106</v>
       </c>
@@ -1982,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3">
       <c r="B135" s="27" t="s">
         <v>107</v>
       </c>
@@ -1990,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3">
       <c r="B136" s="27" t="s">
         <v>108</v>
       </c>
@@ -1998,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3">
       <c r="B137" s="27" t="s">
         <v>109</v>
       </c>
@@ -2006,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3">
       <c r="B138" s="27" t="s">
         <v>110</v>
       </c>
@@ -2014,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3">
       <c r="B139" s="27" t="s">
         <v>111</v>
       </c>
@@ -2022,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3">
       <c r="B140" s="27" t="s">
         <v>112</v>
       </c>
@@ -2030,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3">
       <c r="B141" s="27" t="s">
         <v>113</v>
       </c>
@@ -2038,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3">
       <c r="B142" s="27" t="s">
         <v>114</v>
       </c>
@@ -2046,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3">
       <c r="B143" s="27" t="s">
         <v>115</v>
       </c>
@@ -2054,7 +2052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3">
       <c r="B144" s="27" t="s">
         <v>116</v>
       </c>
@@ -2062,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3">
       <c r="B145" s="27" t="s">
         <v>117</v>
       </c>
@@ -2070,7 +2068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="6:6">
       <c r="F165" s="2"/>
     </row>
   </sheetData>
@@ -2156,7 +2154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2164,7 +2162,7 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
@@ -2172,7 +2170,7 @@
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="20" customFormat="1">
       <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
@@ -2186,7 +2184,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2200,7 +2198,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2211,7 +2209,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>49</v>
       </c>
@@ -2219,7 +2217,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="D5" t="s">
         <v>89</v>
       </c>
@@ -2231,7 +2229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O16"/>
   <sheetViews>
@@ -2239,12 +2237,12 @@
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="20" customFormat="1">
       <c r="B1" s="20" t="s">
         <v>118</v>
       </c>
@@ -2288,7 +2286,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="20" t="s">
         <v>103</v>
       </c>
@@ -2335,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="20" t="s">
         <v>104</v>
       </c>
@@ -2382,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="20" t="s">
         <v>105</v>
       </c>
@@ -2429,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="20" t="s">
         <v>106</v>
       </c>
@@ -2476,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="20" t="s">
         <v>107</v>
       </c>
@@ -2523,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="20" t="s">
         <v>108</v>
       </c>
@@ -2570,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="20" t="s">
         <v>109</v>
       </c>
@@ -2617,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="20" t="s">
         <v>110</v>
       </c>
@@ -2664,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="20" t="s">
         <v>111</v>
       </c>
@@ -2711,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="20" t="s">
         <v>112</v>
       </c>
@@ -2758,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="20" t="s">
         <v>113</v>
       </c>
@@ -2805,7 +2803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="20" t="s">
         <v>114</v>
       </c>
@@ -2852,7 +2850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="20" t="s">
         <v>115</v>
       </c>
@@ -2899,7 +2897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="20" t="s">
         <v>116</v>
       </c>
@@ -2946,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="20" t="s">
         <v>117</v>
       </c>

</xml_diff>